<commit_message>
feat: added test cases to Excel file
</commit_message>
<xml_diff>
--- a/test cases.xlsx
+++ b/test cases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10332" tabRatio="602" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10332" tabRatio="602"/>
   </bookViews>
   <sheets>
     <sheet name="Smoke Test Check-list" sheetId="6" r:id="rId1"/>
@@ -14,18 +14,18 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Critical Path Test'!$A$1:$F$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$67</definedName>
-    <definedName name="Z_076E216B_083E_4703_B60A_D13E6F869911_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$67</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$71</definedName>
+    <definedName name="Z_076E216B_083E_4703_B60A_D13E6F869911_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$71</definedName>
     <definedName name="Z_082914DE_9BEF_4308_9DE4_FA5DD1E31CC1_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!#REF!</definedName>
     <definedName name="Z_08B424B6_41BA_4DCE_BBD3_51945A45BE64_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$I$1:$I$1</definedName>
-    <definedName name="Z_0D273C76_6366_4301_AD32_22F4637E447E_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$67</definedName>
-    <definedName name="Z_0D27DA27_04C0_4697_AF88_60E49E3B520D_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$67</definedName>
+    <definedName name="Z_0D273C76_6366_4301_AD32_22F4637E447E_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$71</definedName>
+    <definedName name="Z_0D27DA27_04C0_4697_AF88_60E49E3B520D_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$71</definedName>
     <definedName name="Z_10742954_85DC_41BF_95C5_974CA284DD52_.wvu.FilterData" localSheetId="3" hidden="1">'Critical Path Test'!$A$1:$F$3</definedName>
     <definedName name="Z_116720F1_EEAC_4D84_BB27_D5A6A3F3078E_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!#REF!</definedName>
     <definedName name="Z_150981C5_D6BA_4460_9AE5_D129261C65C2_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$I$1:$I$1</definedName>
     <definedName name="Z_1521F199_6F51_4B96_AF69_DFD6E5A59948_.wvu.FilterData" localSheetId="3" hidden="1">'Critical Path Test'!$A$1:$F$3</definedName>
-    <definedName name="Z_155A2797_6A59_4BC9_9418_C86809FE2A76_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$67</definedName>
-    <definedName name="Z_1642222A_E978_431B_A276_AC11260CDF6A_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$67</definedName>
+    <definedName name="Z_155A2797_6A59_4BC9_9418_C86809FE2A76_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$71</definedName>
+    <definedName name="Z_1642222A_E978_431B_A276_AC11260CDF6A_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$71</definedName>
     <definedName name="Z_18E12BE6_5BE0_4DEE_9AD7_0A6C822D5D1E_.wvu.FilterData" localSheetId="3" hidden="1">'Critical Path Test'!$A$1:$F$3</definedName>
     <definedName name="Z_190A9DA7_F7A3_11D6_8372_00A0C9A45549_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!#REF!</definedName>
     <definedName name="Z_190A9DAC_F7A3_11D6_8372_00A0C9A45549_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!#REF!</definedName>
@@ -35,53 +35,53 @@
     <definedName name="Z_1B89DDD6_9D67_11D6_83FA_0003470A98B2_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$I$1:$I$1</definedName>
     <definedName name="Z_1B89DDDA_9D67_11D6_83FA_0003470A98B2_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$I$1:$I$1</definedName>
     <definedName name="Z_1B8AE6A8_7CB5_4C58_B840_0E7BE1029C49_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$B$1:$B$1</definedName>
-    <definedName name="Z_1C00113E_A4B5_41F5_A5DE_BDE7D78C755C_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$67</definedName>
-    <definedName name="Z_1C87E219_95E4_4488_A51E_4A020664B1DD_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$67</definedName>
+    <definedName name="Z_1C00113E_A4B5_41F5_A5DE_BDE7D78C755C_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$71</definedName>
+    <definedName name="Z_1C87E219_95E4_4488_A51E_4A020664B1DD_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$71</definedName>
     <definedName name="Z_1CB8DF49_8AC6_4C40_974A_C4C03027F95C_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!#REF!</definedName>
     <definedName name="Z_1F490414_393C_45B4_91E0_1F00E13DEB7A_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$I$1:$I$1</definedName>
     <definedName name="Z_1F6181B7_F2F4_4AC3_83C6_17A6D52430BD_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!#REF!</definedName>
-    <definedName name="Z_20F15AE4_BB0F_4D2F_92CD_6555EFFD634F_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$67</definedName>
-    <definedName name="Z_215F7C28_7EBA_4FFE_8446_E3B3606F5677_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$67</definedName>
-    <definedName name="Z_2534AD3F_F292_40B6_A4A5_4447C5F2D534_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$67</definedName>
+    <definedName name="Z_20F15AE4_BB0F_4D2F_92CD_6555EFFD634F_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$71</definedName>
+    <definedName name="Z_215F7C28_7EBA_4FFE_8446_E3B3606F5677_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$71</definedName>
+    <definedName name="Z_2534AD3F_F292_40B6_A4A5_4447C5F2D534_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$71</definedName>
     <definedName name="Z_25E61601_54D4_4DF5_9420_10EEDDEB8CD0_.wvu.FilterData" localSheetId="3" hidden="1">'Critical Path Test'!$A$1:$F$3</definedName>
     <definedName name="Z_26053C6E_BED6_41EA_8F3E_71A27999119C_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!#REF!</definedName>
     <definedName name="Z_298F2EE3_97E3_11D6_83F5_0003470A98B2_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$I$1:$I$1</definedName>
     <definedName name="Z_298F2EE5_97E3_11D6_83F5_0003470A98B2_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$I$1:$I$1</definedName>
     <definedName name="Z_298F2EE8_97E3_11D6_83F5_0003470A98B2_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$I$1:$I$1</definedName>
     <definedName name="Z_298F2EEA_97E3_11D6_83F5_0003470A98B2_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$I$1:$I$1</definedName>
-    <definedName name="Z_2A0D72AF_A612_4F6A_8DF3_44A4D9105A70_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$67</definedName>
+    <definedName name="Z_2A0D72AF_A612_4F6A_8DF3_44A4D9105A70_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$71</definedName>
     <definedName name="Z_2A7DD623_02F3_4B95_A1D9_047DE55EBDF4_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$B$1:$B$1</definedName>
     <definedName name="Z_2AB83677_E1CF_11D6_8453_0003470A98B2_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!#REF!</definedName>
-    <definedName name="Z_2B5169DB_55BA_4740_B85D_EFCD25EE849A_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$67</definedName>
+    <definedName name="Z_2B5169DB_55BA_4740_B85D_EFCD25EE849A_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$71</definedName>
     <definedName name="Z_2D2F3548_EA47_11D6_8365_00A0C9A45549_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!#REF!</definedName>
     <definedName name="Z_2E86E342_D843_41F1_81B9_004DC563AD09_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!#REF!</definedName>
     <definedName name="Z_3118D002_23F3_4D98_BE60_1D3F51DD9096_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!#REF!</definedName>
-    <definedName name="Z_31351E84_0E49_4F7D_B5E0_670B75EEB0EE_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$67</definedName>
+    <definedName name="Z_31351E84_0E49_4F7D_B5E0_670B75EEB0EE_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$71</definedName>
     <definedName name="Z_316CFC25_EB3C_11D6_8273_009027651E6D_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!#REF!</definedName>
     <definedName name="Z_316CFC27_EB3C_11D6_8273_009027651E6D_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!#REF!</definedName>
-    <definedName name="Z_31B4872D_A493_434A_B894_ADDA078D2553_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$67</definedName>
+    <definedName name="Z_31B4872D_A493_434A_B894_ADDA078D2553_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$71</definedName>
     <definedName name="Z_338074CA_E267_11D6_835F_00A0C9A45549_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!#REF!</definedName>
     <definedName name="Z_33E499A9_C514_4463_9D4F_E656C07E11F3_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$B$1:$B$1</definedName>
     <definedName name="Z_34229D04_7409_4F69_9D94_8AC3B7BE4235_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!#REF!</definedName>
     <definedName name="Z_38DD1442_24D9_4DA6_B8D0_BF77726EC80E_.wvu.FilterData" localSheetId="3" hidden="1">'Critical Path Test'!$A$1:$F$3</definedName>
     <definedName name="Z_3B2FDBA4_87C2_4F65_B9F7_3940A1C730FE_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!#REF!</definedName>
-    <definedName name="Z_3B8911D5_7843_4FC6_9696_0DEF6B150621_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$67</definedName>
+    <definedName name="Z_3B8911D5_7843_4FC6_9696_0DEF6B150621_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$71</definedName>
     <definedName name="Z_3B9C9234_CAD4_4D2F_A608_6EE4D068EA6A_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$I$1:$I$1</definedName>
     <definedName name="Z_3CAF842E_E065_4523_9D51_AF13869D6EB8_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!#REF!</definedName>
-    <definedName name="Z_3CB96B1B_B014_4B85_A883_CCD24970E730_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$67</definedName>
+    <definedName name="Z_3CB96B1B_B014_4B85_A883_CCD24970E730_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$71</definedName>
     <definedName name="Z_3E98E84F_DE56_410D_AA8E_A0C8C093390B_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$B$1:$B$1</definedName>
     <definedName name="Z_3EDD5E42_79E4_11D6_8216_009027651E6D_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$I$1:$I$1</definedName>
     <definedName name="Z_4004633E_3EB7_4A71_9B54_33CE8E2476D0_.wvu.FilterData" localSheetId="3" hidden="1">'Critical Path Test'!$A$1:$F$3</definedName>
     <definedName name="Z_40765E5D_8E4D_4EBD_841D_B3BCC0D26A90_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!#REF!</definedName>
-    <definedName name="Z_4093189C_3129_4D91_950C_4930C9EAAD75_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$67</definedName>
-    <definedName name="Z_409BEDCA_07FB_4362_B5FC_2CCFD1B33BFB_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$67</definedName>
-    <definedName name="Z_4426B116_B740_4CFB_BDED_5285AA879C36_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$67</definedName>
+    <definedName name="Z_4093189C_3129_4D91_950C_4930C9EAAD75_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$71</definedName>
+    <definedName name="Z_409BEDCA_07FB_4362_B5FC_2CCFD1B33BFB_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$71</definedName>
+    <definedName name="Z_4426B116_B740_4CFB_BDED_5285AA879C36_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$71</definedName>
     <definedName name="Z_44EB34BD_5782_42C6_94CC_2811B0118C6F_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$I$1:$I$1</definedName>
     <definedName name="Z_450B48D9_8BF6_44F2_B825_EEFAFBCFA6B0_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!#REF!</definedName>
     <definedName name="Z_45FC9312_D50D_11D6_8257_009027651E6D_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$I$1:$I$1</definedName>
     <definedName name="Z_497CDFBC_BC24_4493_823C_8715DDDB194A_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!#REF!</definedName>
-    <definedName name="Z_49B88D39_760F_49FE_9089_8995DAD8FC78_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$67</definedName>
-    <definedName name="Z_4B0A933D_07FE_4CA2_B4FC_79E22BCB1563_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$67</definedName>
+    <definedName name="Z_49B88D39_760F_49FE_9089_8995DAD8FC78_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$71</definedName>
+    <definedName name="Z_4B0A933D_07FE_4CA2_B4FC_79E22BCB1563_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$71</definedName>
     <definedName name="Z_4BC641D9_44D1_48CA_A2E8_D60FF2D16BA5_.wvu.FilterData" localSheetId="3" hidden="1">'Critical Path Test'!$A$1:$F$3</definedName>
     <definedName name="Z_4BD80E6A_F19B_488D_A100_857C2CB69C3E_.wvu.FilterData" localSheetId="3" hidden="1">'Critical Path Test'!$A$1:$F$3</definedName>
     <definedName name="Z_4BF74373_06CF_11D7_8299_009027651E6D_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!#REF!</definedName>
@@ -96,29 +96,29 @@
     <definedName name="Z_501225BA_B4D2_11D6_8463_009027ED1955_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$I$1:$I$1</definedName>
     <definedName name="Z_5099C3F7_31CA_4231_82FB_8CA3A0F4BB16_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!#REF!</definedName>
     <definedName name="Z_55F705DA_03EF_49BA_B354_F86FDA6069F7_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!#REF!</definedName>
-    <definedName name="Z_5735CCC5_D030_4C1D_BB3B_07EB54974141_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$67</definedName>
+    <definedName name="Z_5735CCC5_D030_4C1D_BB3B_07EB54974141_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$71</definedName>
     <definedName name="Z_58565E39_C845_45B2_ADE0_C5D6F122D12F_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!#REF!</definedName>
-    <definedName name="Z_5962F1E5_A319_4093_BAFC_598A35290AF6_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$67</definedName>
+    <definedName name="Z_5962F1E5_A319_4093_BAFC_598A35290AF6_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$71</definedName>
     <definedName name="Z_5993E09E_C0E9_42E0_992F_E19006AFF5B2_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!#REF!</definedName>
-    <definedName name="Z_5A6D0686_9738_46B6_B40A_F9C1292DDE09_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$67</definedName>
+    <definedName name="Z_5A6D0686_9738_46B6_B40A_F9C1292DDE09_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$71</definedName>
     <definedName name="Z_5F0BDA38_467D_43D0_AFF6_BD58C644CA07_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!#REF!</definedName>
     <definedName name="Z_5F45B89A_43AE_47CB_B4C3_C5F41EE6F1B4_.wvu.FilterData" localSheetId="3" hidden="1">'Critical Path Test'!$A$1:$F$3</definedName>
     <definedName name="Z_610E9A8B_D744_406E_9233_462E4B2D977E_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!#REF!</definedName>
-    <definedName name="Z_61B848E0_F845_4930_B6B1_AE54A626711C_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$67</definedName>
+    <definedName name="Z_61B848E0_F845_4930_B6B1_AE54A626711C_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$71</definedName>
     <definedName name="Z_63383682_6E23_11D6_82E5_00A0C9A45549_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$I$1:$I$1</definedName>
     <definedName name="Z_63383684_6E23_11D6_82E5_00A0C9A45549_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$I$1:$I$1</definedName>
     <definedName name="Z_63383686_6E23_11D6_82E5_00A0C9A45549_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$I$1:$I$1</definedName>
     <definedName name="Z_64A375AD_C551_49C2_B580_75A3A5EDC174_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!#REF!</definedName>
     <definedName name="Z_65DF2B85_7FF1_4768_B5D5_7805E9E94385_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!#REF!</definedName>
     <definedName name="Z_65EC132F_6304_4D16_AF47_33FB3C6D1982_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!#REF!</definedName>
-    <definedName name="Z_6840A0D3_58BA_4F3A_9D23_8EF68E28FCD7_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$67</definedName>
-    <definedName name="Z_6B0F124C_D4CA_4142_B823_93138A450C5A_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$67</definedName>
+    <definedName name="Z_6840A0D3_58BA_4F3A_9D23_8EF68E28FCD7_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$71</definedName>
+    <definedName name="Z_6B0F124C_D4CA_4142_B823_93138A450C5A_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$71</definedName>
     <definedName name="Z_6C751807_9E2D_11D6_83FB_0003470A98B2_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$I$1:$I$1</definedName>
     <definedName name="Z_7063472E_EF65_4BD0_830D_4FD26C29AE7E_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$B$1:$B$1</definedName>
     <definedName name="Z_70DEF7F0_FC23_4363_9224_C5EA941C5550_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$B$1:$B$1</definedName>
     <definedName name="Z_7166D88D_13B1_445A_9C1B_1D44F9C0FFC4_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$I$1:$I$1</definedName>
     <definedName name="Z_726523F9_B36A_4B91_B07D_11A835D68B55_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!#REF!</definedName>
-    <definedName name="Z_728C8D61_6AD0_41BA_9B1A_1FECB7699DC1_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$67</definedName>
+    <definedName name="Z_728C8D61_6AD0_41BA_9B1A_1FECB7699DC1_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$71</definedName>
     <definedName name="Z_74226AEF_5AD7_4164_9E49_0568DB2D1C02_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!#REF!</definedName>
     <definedName name="Z_74C15D45_BF0F_11D6_8333_00A0C9A45549_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$I$1:$I$1</definedName>
     <definedName name="Z_7675A241_C48A_11D6_8476_009027ED1955_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$I$1:$I$1</definedName>
@@ -136,10 +136,10 @@
     <definedName name="Z_7BB5586D_F8DA_4286_B856_F6D48BFC67EC_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$I$1:$I$1</definedName>
     <definedName name="Z_7CD7CA53_BB22_11D6_841E_0003470A98B2_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$I$1:$I$1</definedName>
     <definedName name="Z_7CD7CA55_BB22_11D6_841E_0003470A98B2_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$I$1:$I$1</definedName>
-    <definedName name="Z_7DB709A3_B05C_4BDF_9940_7B4164498565_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$67</definedName>
-    <definedName name="Z_7F43198E_AEB4_4B2B_A204_B31C1DAF0612_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$67</definedName>
+    <definedName name="Z_7DB709A3_B05C_4BDF_9940_7B4164498565_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$71</definedName>
+    <definedName name="Z_7F43198E_AEB4_4B2B_A204_B31C1DAF0612_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$71</definedName>
     <definedName name="Z_7FEEB23E_9B4F_4161_A01D_4E0E62555D50_.wvu.FilterData" localSheetId="3" hidden="1">'Critical Path Test'!$A$1:$F$3</definedName>
-    <definedName name="Z_7FF35F33_9949_4D85_9EC7_D06D3DF0FD09_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$67</definedName>
+    <definedName name="Z_7FF35F33_9949_4D85_9EC7_D06D3DF0FD09_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$71</definedName>
     <definedName name="Z_82666A53_BFCF_11D6_8472_009027ED1955_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$I$1:$I$1</definedName>
     <definedName name="Z_82CB83AA_FB92_11D6_8376_00A0C9A45549_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!#REF!</definedName>
     <definedName name="Z_835F3151_9402_11D6_8434_009027ED1955_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$I$1:$I$1</definedName>
@@ -152,19 +152,19 @@
     <definedName name="Z_87B21F02_EFDF_11D6_8277_009027651E6D_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!#REF!</definedName>
     <definedName name="Z_8A3AABE0_F8AF_4EAE_8F30_89A1B8FEDCBC_.wvu.FilterData" localSheetId="3" hidden="1">'Critical Path Test'!$A$1:$F$3</definedName>
     <definedName name="Z_8B1E9C6C_6EE0_11D6_82E6_00A0C9A45549_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$I$1:$I$1</definedName>
-    <definedName name="Z_8BC8433F_BD44_42F6_ABF1_D600CDA6814E_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$67</definedName>
-    <definedName name="Z_8EF7F386_5E51_4F8D_A999_0ADCED76F401_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$67</definedName>
+    <definedName name="Z_8BC8433F_BD44_42F6_ABF1_D600CDA6814E_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$71</definedName>
+    <definedName name="Z_8EF7F386_5E51_4F8D_A999_0ADCED76F401_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$71</definedName>
     <definedName name="Z_91C9BCC0_E2CE_45C1_BC0A_46F0C7B3DD86_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$I$1:$I$1</definedName>
-    <definedName name="Z_9355331B_2DDD_4EC1_A731_4FBA46A44FB0_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$67</definedName>
-    <definedName name="Z_946F5E20_9204_4B29_AB65_FC542EF09444_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$67</definedName>
-    <definedName name="Z_9476BCEB_3128_4E71_AFAC_36F823E78B58_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$67</definedName>
+    <definedName name="Z_9355331B_2DDD_4EC1_A731_4FBA46A44FB0_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$71</definedName>
+    <definedName name="Z_946F5E20_9204_4B29_AB65_FC542EF09444_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$71</definedName>
+    <definedName name="Z_9476BCEB_3128_4E71_AFAC_36F823E78B58_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$71</definedName>
     <definedName name="Z_952813C8_3005_4385_824B_16A14AD6A965_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!#REF!</definedName>
-    <definedName name="Z_95B1AE55_5A09_43C3_B842_92A6A8CBB4FF_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$67</definedName>
-    <definedName name="Z_9DB4E31D_4D0C_4D4A_9B0E_5CB499C8FCE0_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$67</definedName>
+    <definedName name="Z_95B1AE55_5A09_43C3_B842_92A6A8CBB4FF_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$71</definedName>
+    <definedName name="Z_9DB4E31D_4D0C_4D4A_9B0E_5CB499C8FCE0_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$71</definedName>
     <definedName name="Z_9DC25E1A_7C77_11D6_8428_009027ED1955_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$I$1:$I$1</definedName>
     <definedName name="Z_9E0603F2_17C3_46DE_96C7_2B055B19C810_.wvu.FilterData" localSheetId="3" hidden="1">'Critical Path Test'!$A$1:$F$3</definedName>
-    <definedName name="Z_9E29624A_918B_446F_BAE8_4FE6993177DA_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$72</definedName>
-    <definedName name="Z_9F54D8CA_F7CA_4FBD_A510_4B321446D110_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$67</definedName>
+    <definedName name="Z_9E29624A_918B_446F_BAE8_4FE6993177DA_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$76</definedName>
+    <definedName name="Z_9F54D8CA_F7CA_4FBD_A510_4B321446D110_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$71</definedName>
     <definedName name="Z_A03BC55B_97AE_49A8_AC72_55FE44CD9CC7_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!#REF!</definedName>
     <definedName name="Z_A0E0EC78_49C7_4C2F_85EC_C53F902DEEAF_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$I$1:$I$1</definedName>
     <definedName name="Z_A21F3490_E19A_11D6_835E_00A0C9A45549_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!#REF!</definedName>
@@ -172,38 +172,38 @@
     <definedName name="Z_A21F3497_E19A_11D6_835E_00A0C9A45549_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!#REF!</definedName>
     <definedName name="Z_A21F3499_E19A_11D6_835E_00A0C9A45549_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!#REF!</definedName>
     <definedName name="Z_A292D6EF_6D62_4E4C_858F_8AF879C77534_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!#REF!</definedName>
-    <definedName name="Z_A2CDC5AD_2424_46FB_B14B_520BC4052840_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$67</definedName>
-    <definedName name="Z_A31F803A_536A_4424_9C72_1DA9E3728743_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$67</definedName>
-    <definedName name="Z_A3A8C529_06E3_4F0D_A55A_18470A16A280_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$67</definedName>
-    <definedName name="Z_A49D00B0_1CA2_4CFF_9CE8_E2870820CBFE_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$67</definedName>
-    <definedName name="Z_A5865E10_F199_45F2_9978_AB2FD62E3988_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$67</definedName>
+    <definedName name="Z_A2CDC5AD_2424_46FB_B14B_520BC4052840_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$71</definedName>
+    <definedName name="Z_A31F803A_536A_4424_9C72_1DA9E3728743_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$71</definedName>
+    <definedName name="Z_A3A8C529_06E3_4F0D_A55A_18470A16A280_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$71</definedName>
+    <definedName name="Z_A49D00B0_1CA2_4CFF_9CE8_E2870820CBFE_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$71</definedName>
+    <definedName name="Z_A5865E10_F199_45F2_9978_AB2FD62E3988_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$71</definedName>
     <definedName name="Z_A7EE37B0_1621_46A3_821F_17E9F67DE25E_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$I$1:$I$1</definedName>
-    <definedName name="Z_A85A58A3_C882_49B8_B616_6650AF7312E1_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$67</definedName>
+    <definedName name="Z_A85A58A3_C882_49B8_B616_6650AF7312E1_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$71</definedName>
     <definedName name="Z_A9C99871_C550_11D6_8477_009027ED1955_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$I$1:$I$1</definedName>
     <definedName name="Z_A9C99875_C550_11D6_8477_009027ED1955_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$I$1:$I$1</definedName>
-    <definedName name="Z_AAD7CBFE_CAFD_4DBE_90C8_44A2880265AF_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$67</definedName>
-    <definedName name="Z_AB29D946_56C9_4D46_AC18_AAAB8BB36ED8_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$67</definedName>
-    <definedName name="Z_AC386442_F892_40E2_8D4D_E181578B2D5A_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$67</definedName>
+    <definedName name="Z_AAD7CBFE_CAFD_4DBE_90C8_44A2880265AF_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$71</definedName>
+    <definedName name="Z_AB29D946_56C9_4D46_AC18_AAAB8BB36ED8_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$71</definedName>
+    <definedName name="Z_AC386442_F892_40E2_8D4D_E181578B2D5A_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$71</definedName>
     <definedName name="Z_AC84E601_FDE2_4D6C_8497_F05D4116AFED_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!#REF!</definedName>
-    <definedName name="Z_B0F3A36C_DF31_41C4_B3EB_657F870836E7_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$67</definedName>
+    <definedName name="Z_B0F3A36C_DF31_41C4_B3EB_657F870836E7_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$71</definedName>
     <definedName name="Z_B11D1D33_BCFF_4CB8_B47A_78C107A7D7C5_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$I$1:$I$1</definedName>
     <definedName name="Z_B1201F92_721E_11D6_83D1_0003470A98B2_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$I$1:$I$1</definedName>
     <definedName name="Z_B1201F94_721E_11D6_83D1_0003470A98B2_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$I$1:$I$1</definedName>
     <definedName name="Z_B3376F5F_9342_4FE3_B88E_37813E471B56_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!#REF!</definedName>
     <definedName name="Z_B34DDB5F_F5C1_4B53_A698_ED068265A80A_.wvu.FilterData" localSheetId="3" hidden="1">'Critical Path Test'!$A$1:$F$3</definedName>
-    <definedName name="Z_B3B78B55_F23F_4975_8147_E339DE956271_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$67</definedName>
+    <definedName name="Z_B3B78B55_F23F_4975_8147_E339DE956271_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$71</definedName>
     <definedName name="Z_B572C60E_2FE3_4505_8D16_F47BC00CAD64_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$I$1:$I$1</definedName>
     <definedName name="Z_B6B3B788_0059_11D7_91C5_009027ED19A4_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!#REF!</definedName>
-    <definedName name="Z_B6EC6533_326F_4A12_8620_F81E37B51C4F_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$67</definedName>
-    <definedName name="Z_BA07A066_46E1_4976_8B94_1EB8F7BBD358_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$67</definedName>
-    <definedName name="Z_BA710EE8_1DE3_4C75_A992_DB0C26B41697_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$67</definedName>
-    <definedName name="Z_BBE3BD38_8D06_4C53_9033_E19DED6AD8E5_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$67</definedName>
-    <definedName name="Z_BE576D3A_46D1_4F51_BA35_C79DF66104A0_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$67</definedName>
-    <definedName name="Z_BE6B98F0_BC28_4858_82AE_C3EFE6A6AA8E_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$67</definedName>
-    <definedName name="Z_BE871476_FA83_4225_9B8E_440E3E381E1E_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$67</definedName>
-    <definedName name="Z_C204AC43_4420_4F08_AD56_0AE71F5E582E_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$67</definedName>
+    <definedName name="Z_B6EC6533_326F_4A12_8620_F81E37B51C4F_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$71</definedName>
+    <definedName name="Z_BA07A066_46E1_4976_8B94_1EB8F7BBD358_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$71</definedName>
+    <definedName name="Z_BA710EE8_1DE3_4C75_A992_DB0C26B41697_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$71</definedName>
+    <definedName name="Z_BBE3BD38_8D06_4C53_9033_E19DED6AD8E5_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$71</definedName>
+    <definedName name="Z_BE576D3A_46D1_4F51_BA35_C79DF66104A0_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$71</definedName>
+    <definedName name="Z_BE6B98F0_BC28_4858_82AE_C3EFE6A6AA8E_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$71</definedName>
+    <definedName name="Z_BE871476_FA83_4225_9B8E_440E3E381E1E_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$71</definedName>
+    <definedName name="Z_C204AC43_4420_4F08_AD56_0AE71F5E582E_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$71</definedName>
     <definedName name="Z_C417C51E_8A62_4805_A169_0AEB5301D042_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$B$1:$B$1</definedName>
-    <definedName name="Z_C4A79BA5_AE70_444E_A37D_87EDC872940C_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$67</definedName>
+    <definedName name="Z_C4A79BA5_AE70_444E_A37D_87EDC872940C_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$71</definedName>
     <definedName name="Z_C92840F2_F4E8_4E7E_BD26_3E48E4767E5B_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!#REF!</definedName>
     <definedName name="Z_C92CF23E_DF42_11D6_8260_009027651E6D_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!#REF!</definedName>
     <definedName name="Z_C92CF248_DF42_11D6_8260_009027651E6D_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!#REF!</definedName>
@@ -213,7 +213,7 @@
     <definedName name="Z_CB548DF9_F6DC_11D6_8371_00A0C9A45549_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!#REF!</definedName>
     <definedName name="Z_CB88F70C_24C4_4FAE_933B_ADD49CE937DF_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!#REF!</definedName>
     <definedName name="Z_CD0A5058_1296_4D68_8710_49F9D884EDE7_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!#REF!</definedName>
-    <definedName name="Z_CEF471D2_B5D2_4065_AF99_BD425F204B07_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$67</definedName>
+    <definedName name="Z_CEF471D2_B5D2_4065_AF99_BD425F204B07_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$71</definedName>
     <definedName name="Z_CFB3C796_8AEC_4B3E_A039_80D09F3D2C5B_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!#REF!</definedName>
     <definedName name="Z_D0177061_A217_49C2_8125_93EF8BE93AE1_.wvu.FilterData" localSheetId="3" hidden="1">'Critical Path Test'!$A$1:$F$3</definedName>
     <definedName name="Z_D066A59E_81DA_11D6_842C_009027ED1955_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$I$1:$I$1</definedName>
@@ -232,7 +232,7 @@
     <definedName name="Z_D066A69B_81DA_11D6_842C_009027ED1955_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$I$1:$I$1</definedName>
     <definedName name="Z_D066A6A2_81DA_11D6_842C_009027ED1955_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$I$1:$I$1</definedName>
     <definedName name="Z_D066A6A6_81DA_11D6_842C_009027ED1955_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$I$1:$I$1</definedName>
-    <definedName name="Z_D09BC2D4_A8FB_4A96_980F_AAAAC7224F56_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$67</definedName>
+    <definedName name="Z_D09BC2D4_A8FB_4A96_980F_AAAAC7224F56_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$71</definedName>
     <definedName name="Z_D12518D6_E4AE_457E_AA12_F4C2DDC1C2D1_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!#REF!</definedName>
     <definedName name="Z_D338C480_DBA1_11D6_8447_0003470A98B2_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!#REF!</definedName>
     <definedName name="Z_D338C483_DBA1_11D6_8447_0003470A98B2_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!#REF!</definedName>
@@ -241,8 +241,8 @@
     <definedName name="Z_D84DD29E_BF30_11D6_8471_009027ED1955_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$I$1:$I$1</definedName>
     <definedName name="Z_D84DD2A0_BF30_11D6_8471_009027ED1955_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$I$1:$I$1</definedName>
     <definedName name="Z_D84DD2A3_BF30_11D6_8471_009027ED1955_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$I$1:$I$1</definedName>
-    <definedName name="Z_DA439189_9374_4891_8465_D08760D6F042_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$67</definedName>
-    <definedName name="Z_DB0364DE_3D33_44A9_930D_3F40EABC0A74_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$67</definedName>
+    <definedName name="Z_DA439189_9374_4891_8465_D08760D6F042_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$71</definedName>
+    <definedName name="Z_DB0364DE_3D33_44A9_930D_3F40EABC0A74_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$71</definedName>
     <definedName name="Z_DBE7F2B1_9256_43D2_BB21_88117D04D3F6_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!#REF!</definedName>
     <definedName name="Z_DDDC66C1_AB8D_4A01_8BEA_37527371B671_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$I$1:$I$1</definedName>
     <definedName name="Z_E0A36D26_A7D1_43E8_B670_231D68B72352_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!#REF!</definedName>
@@ -265,8 +265,8 @@
     <definedName name="Z_F079D6D2_6FAA_11D6_82E7_00A0C9A45549_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$I$1:$I$1</definedName>
     <definedName name="Z_F4109F33_260A_4792_B916_486D7E09C187_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$B$1:$B$1</definedName>
     <definedName name="Z_F84AE8F5_DB84_11D6_8447_0003470A98B2_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!#REF!</definedName>
-    <definedName name="Z_FC4B7E83_EDFB_4099_9166_7E4E1FFA01AF_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$67</definedName>
-    <definedName name="Z_FE3D740C_F87C_4E94_88EC_1F9D8F95903F_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$67</definedName>
+    <definedName name="Z_FC4B7E83_EDFB_4099_9166_7E4E1FFA01AF_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$71</definedName>
+    <definedName name="Z_FE3D740C_F87C_4E94_88EC_1F9D8F95903F_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$A$1:$H$71</definedName>
     <definedName name="Z_FE99B5D3_94A3_4B2A_BE2E_6FB0B152125A_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!$I$1:$I$1</definedName>
     <definedName name="Z_FF0C638A_6B57_4CDB_9627_F21E5F8E958C_.wvu.FilterData" localSheetId="1" hidden="1">'Smoke Test'!#REF!</definedName>
   </definedNames>
@@ -275,7 +275,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="122">
   <si>
     <t>Requirements No.</t>
   </si>
@@ -466,12 +466,6 @@
     <t>21</t>
   </si>
   <si>
-    <t xml:space="preserve">CLI </t>
-  </si>
-  <si>
-    <t>Start</t>
-  </si>
-  <si>
     <t>Application DOES NOT start when an incorrect command is entered</t>
   </si>
   <si>
@@ -493,8 +487,180 @@
     <t xml:space="preserve">The app is started by entering a command containing: the path for the HTML output, the path for the CSV output and the starting directory  </t>
   </si>
   <si>
-    <t xml:space="preserve">1.open the console
-2. </t>
+    <t>TS1.TC1</t>
+  </si>
+  <si>
+    <t>TS1.TC2</t>
+  </si>
+  <si>
+    <t>CLI</t>
+  </si>
+  <si>
+    <t>Starting the app with missing HTML path</t>
+  </si>
+  <si>
+    <t>TS1.TC3</t>
+  </si>
+  <si>
+    <t>1.open the console
+2. enter the command “java -jar AudioCataloger.jar [DuplicatesOnly]  CsvOutputFileName StartingDirectory1 [... StartingDirectoryN]”</t>
+  </si>
+  <si>
+    <t>UR-1.1, DS-2.2, DS-3.1</t>
+  </si>
+  <si>
+    <t>Starting the app with missing CSV path</t>
+  </si>
+  <si>
+    <t>Starting the app with missing directory path</t>
+  </si>
+  <si>
+    <t>The usage message appears: “Usage: java -jar AudioCataloger.jar [DuplicatesOnly] HtmlOutputFileName CsvOutputFileName StartingDirectory1 [... StartingDirectoryN]”. Informing the user on the necessary parameters for using the application</t>
+  </si>
+  <si>
+    <t>The app is started as described in TS1.TC1 except the path for the HTML output is omitted</t>
+  </si>
+  <si>
+    <t>The app is started as described in TS1.TC1 except the path for the CSV output is omitted</t>
+  </si>
+  <si>
+    <t>The app is started as described in TS1.TC1 except the path for the (starting) directory is omitted</t>
+  </si>
+  <si>
+    <t>Stopping the app</t>
+  </si>
+  <si>
+    <t>TS2.TC2</t>
+  </si>
+  <si>
+    <t>TS2.TC1</t>
+  </si>
+  <si>
+    <t>The application shuts down</t>
+  </si>
+  <si>
+    <t>TS2.TC3</t>
+  </si>
+  <si>
+    <t>TS1.TC4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The program outputs a readable HTML file and a coresponding editable CSV file based on the information from the directory. The paths to each file are displaced in the console. </t>
+  </si>
+  <si>
+    <t>1. Having executed previous cases in test suite 
+2. press the CTRL and C keys at the same time</t>
+  </si>
+  <si>
+    <t>HTML output</t>
+  </si>
+  <si>
+    <t>HTML output is tested for accuracy, readability and viewablity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">An HTML page opens up showing a catalouge of the audio files in the directory in a readable format. The files listed on the page should match the actual audio files in the directory. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Audio Cataloger </t>
+  </si>
+  <si>
+    <t>1. go to the path for the CSV file from TS.TC1 
+2. Open the file in 
+3. Edit the file+D4:F4
+4. Open the HTML file viewed in T1.TC2 and see if the HTML page contains the edits commited to the CSV file  
+5. Compare to the screenshot made in TS.TC2 and document</t>
+  </si>
+  <si>
+    <t>View with HTML</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Editing CSV </t>
+  </si>
+  <si>
+    <t>CSV editor</t>
+  </si>
+  <si>
+    <t>TS1.TC5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Testing for changes to catalogue </t>
+  </si>
+  <si>
+    <t>CSV output is tested to see if it can be edited and is intuitive to edit</t>
+  </si>
+  <si>
+    <t>HTML output is tested to see if the changes made to the CSV file in the editor effected the catalouge in a predictable manner</t>
+  </si>
+  <si>
+    <t>1. go to the HTML file generated in TS.TC1 
+2. Open the file 
+3. Save a screenshot of the HTML output</t>
+  </si>
+  <si>
+    <t>Parameters in Brackets are optional. Will be left out for smoke testing. Assuming a full path is not specified HTML and CSV should be in the same directory as the application.</t>
+  </si>
+  <si>
+    <t>File saves normally and does not crash the application</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. go to the  the CSV file generated in TS.TC1 
+2. Open the file in Excel or another editor of choice
+3. Edit the file by deleting one item, altering one item and adding one item 
+4. Save the CSV file and close out of the editor
+</t>
+  </si>
+  <si>
+    <t>Name of one audio file should be deleted, another name should be altered and a new name should appear</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. go to the HTML file generated in TS.TC1 
+2. Open the file 
+3. compare the current HTML output to the screenshot taken in TS1.TC2 </t>
+  </si>
+  <si>
+    <t>1.open the console
+2. enter the command “java -jar AudioCataloger.jar [DuplicatesOnly] HtmlOutputFileName StartingDirectory1 [... StartingDirectoryN]”</t>
+  </si>
+  <si>
+    <t>1.Populate a directory with audio files (mp3, flac, wav, ogg, wma) up to 2 GB in size
+2. open the console
+3. enter the command “java -jar AudioCataloger.jar [DuplicatesOnly] HtmlOutputFileName CsvOutputFileName StartingDirectory1 [... StartingDirectoryN]”</t>
+  </si>
+  <si>
+    <t>starting the app with a non-existant directory path</t>
+  </si>
+  <si>
+    <t>1.open the console
+2. enter the command “java -jar AudioCataloger.jar [DuplicatesOnly] HtmlOutputFileName StartingDirectory1 [... StartingDirectoryN]” but with the path for the starting directory being one that does not exist in your system</t>
+  </si>
+  <si>
+    <t>The app is started as described in TS1.TC1 except the path for the (starting) directory points to a directory that does not exist</t>
+  </si>
+  <si>
+    <t>The error message appears: “The following directory is not found or is inaccessible: {full path}”; Informing the user that the path does not exist</t>
+  </si>
+  <si>
+    <t>This is for uncorrupted files. Corrupt files tested later</t>
+  </si>
+  <si>
+    <t>Working with corrupted files</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Audio Catalouger  </t>
+  </si>
+  <si>
+    <t>TC3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">App is tested to see if it doesn't crash while processing a corrupt file </t>
+  </si>
+  <si>
+    <t>1. Find a corrupted audio file on the internet
+2. Place it in your directory 
+3. enter the command “java -jar AudioCataloger.jar [DuplicatesOnly] HtmlOutputFileName StartingDirectory1 [... StartingDirectoryN]”</t>
+  </si>
+  <si>
+    <t>The application should not crash</t>
   </si>
 </sst>
 </file>
@@ -707,7 +873,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -788,6 +954,9 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1175,8 +1344,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:I25" totalsRowShown="0" headerRowDxfId="13" dataDxfId="11" headerRowBorderDxfId="12" tableBorderDxfId="10" totalsRowBorderDxfId="9">
-  <autoFilter ref="A1:I25"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:I29" totalsRowShown="0" headerRowDxfId="13" dataDxfId="11" headerRowBorderDxfId="12" tableBorderDxfId="10" totalsRowBorderDxfId="9">
+  <autoFilter ref="A1:I29"/>
   <tableColumns count="9">
     <tableColumn id="1" name="No." dataDxfId="8"/>
     <tableColumn id="2" name="Requirements No." dataDxfId="7"/>
@@ -1481,8 +1650,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:A23"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1534,7 +1703,7 @@
         <v>12</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D3" s="14"/>
       <c r="E3" s="3"/>
@@ -1750,7 +1919,7 @@
         <v>41</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D19" s="14"/>
       <c r="E19" s="3"/>
@@ -1796,7 +1965,7 @@
     </row>
     <row r="23" spans="1:5" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>53</v>
@@ -1945,10 +2114,10 @@
   <sheetPr codeName="Sheet4">
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:I44"/>
+  <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="64" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" zoomScaleSheetLayoutView="64" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1978,13 +2147,13 @@
         <v>3</v>
       </c>
       <c r="E1" s="17" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F1" s="17" t="s">
         <v>4</v>
       </c>
       <c r="G1" s="17" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H1" s="17" t="s">
         <v>5</v>
@@ -1993,128 +2162,278 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="3" customFormat="1" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" s="3" customFormat="1" ht="145.19999999999999" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
-        <v>7</v>
+        <v>70</v>
       </c>
       <c r="B2" s="20" t="s">
         <v>12</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>63</v>
+        <v>94</v>
       </c>
       <c r="D2" s="20" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="E2" s="20" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F2" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="H2" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="I2" s="21" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="3" customFormat="1" ht="66" x14ac:dyDescent="0.25">
+      <c r="A3" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="B3" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="E3" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="F3" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="G3" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="H3" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="I3" s="27" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="3" customFormat="1" ht="118.8" x14ac:dyDescent="0.25">
+      <c r="A4" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="D4" s="25" t="s">
+        <v>98</v>
+      </c>
+      <c r="E4" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="F4" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="G4" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="H4" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="I4" s="27"/>
+    </row>
+    <row r="5" spans="1:9" s="3" customFormat="1" ht="66" x14ac:dyDescent="0.25">
+      <c r="A5" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>94</v>
+      </c>
+      <c r="D5" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="E5" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="F5" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="G5" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="H5" s="25" t="s">
+        <v>107</v>
+      </c>
+      <c r="I5" s="27"/>
+    </row>
+    <row r="6" spans="1:9" s="3" customFormat="1" ht="118.8" x14ac:dyDescent="0.25">
+      <c r="A6" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="B6" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="D6" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="H2" s="20"/>
-      <c r="I2" s="21"/>
-    </row>
-    <row r="3" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="22"/>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="26"/>
-    </row>
-    <row r="4" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="22"/>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="26"/>
-    </row>
-    <row r="5" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="22"/>
-      <c r="B5" s="24"/>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="24"/>
-      <c r="H5" s="24"/>
-      <c r="I5" s="26"/>
-    </row>
-    <row r="6" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="22"/>
-      <c r="B6" s="24"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="24"/>
+      <c r="E6" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="F6" s="24" t="s">
+        <v>95</v>
+      </c>
+      <c r="G6" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="H6" s="24" t="s">
+        <v>86</v>
+      </c>
       <c r="I6" s="26"/>
     </row>
-    <row r="7" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="22"/>
-      <c r="B7" s="24"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="24"/>
+    <row r="7" spans="1:9" s="3" customFormat="1" ht="92.4" x14ac:dyDescent="0.25">
+      <c r="A7" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="B7" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="D7" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="E7" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="F7" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="G7" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="H7" s="24" t="s">
+        <v>79</v>
+      </c>
       <c r="I7" s="26"/>
     </row>
-    <row r="8" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="22"/>
-      <c r="B8" s="24"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="24"/>
+    <row r="8" spans="1:9" s="3" customFormat="1" ht="92.4" x14ac:dyDescent="0.25">
+      <c r="A8" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="B8" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="E8" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="F8" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="G8" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="H8" s="24" t="s">
+        <v>79</v>
+      </c>
       <c r="I8" s="26"/>
     </row>
-    <row r="9" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="22"/>
-      <c r="B9" s="24"/>
-      <c r="C9" s="24"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="24"/>
-      <c r="G9" s="24"/>
-      <c r="H9" s="24"/>
+    <row r="9" spans="1:9" s="3" customFormat="1" ht="92.4" x14ac:dyDescent="0.25">
+      <c r="A9" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="B9" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="D9" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="E9" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="F9" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="G9" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="H9" s="24" t="s">
+        <v>79</v>
+      </c>
       <c r="I9" s="26"/>
     </row>
-    <row r="10" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="22"/>
-      <c r="B10" s="24"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="24"/>
-      <c r="G10" s="24"/>
-      <c r="H10" s="24"/>
-      <c r="I10" s="26"/>
-    </row>
-    <row r="11" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="22"/>
-      <c r="B11" s="24"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="24"/>
+    <row r="10" spans="1:9" ht="96.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="B10" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="D10" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="E10" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="F10" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="G10" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="H10" s="24" t="s">
+        <v>114</v>
+      </c>
+      <c r="I10" s="28"/>
+    </row>
+    <row r="11" spans="1:9" s="3" customFormat="1" ht="92.4" x14ac:dyDescent="0.25">
+      <c r="A11" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="B11" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D11" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="E11" s="24" t="s">
+        <v>116</v>
+      </c>
+      <c r="F11" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="G11" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="H11" s="24" t="s">
+        <v>121</v>
+      </c>
       <c r="I11" s="26"/>
     </row>
     <row r="12" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -2161,7 +2480,7 @@
       <c r="H15" s="24"/>
       <c r="I15" s="26"/>
     </row>
-    <row r="16" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="22"/>
       <c r="B16" s="24"/>
       <c r="C16" s="24"/>
@@ -2172,7 +2491,7 @@
       <c r="H16" s="24"/>
       <c r="I16" s="26"/>
     </row>
-    <row r="17" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="22"/>
       <c r="B17" s="24"/>
       <c r="C17" s="24"/>
@@ -2183,7 +2502,7 @@
       <c r="H17" s="24"/>
       <c r="I17" s="26"/>
     </row>
-    <row r="18" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="22"/>
       <c r="B18" s="24"/>
       <c r="C18" s="24"/>
@@ -2194,7 +2513,7 @@
       <c r="H18" s="24"/>
       <c r="I18" s="26"/>
     </row>
-    <row r="19" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="22"/>
       <c r="B19" s="24"/>
       <c r="C19" s="24"/>
@@ -2261,31 +2580,59 @@
       <c r="I24" s="26"/>
     </row>
     <row r="25" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="23"/>
-      <c r="B25" s="25"/>
-      <c r="C25" s="25"/>
-      <c r="D25" s="25"/>
-      <c r="E25" s="25"/>
-      <c r="F25" s="25"/>
-      <c r="G25" s="25"/>
-      <c r="H25" s="25"/>
-      <c r="I25" s="27"/>
+      <c r="A25" s="22"/>
+      <c r="B25" s="24"/>
+      <c r="C25" s="24"/>
+      <c r="D25" s="24"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="24"/>
+      <c r="G25" s="24"/>
+      <c r="H25" s="24"/>
+      <c r="I25" s="26"/>
     </row>
     <row r="26" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="8"/>
-      <c r="I26" s="15"/>
+      <c r="A26" s="22"/>
+      <c r="B26" s="24"/>
+      <c r="C26" s="24"/>
+      <c r="D26" s="24"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="24"/>
+      <c r="G26" s="24"/>
+      <c r="H26" s="24"/>
+      <c r="I26" s="26"/>
     </row>
     <row r="27" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="8"/>
-      <c r="I27" s="15"/>
+      <c r="A27" s="22"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="24"/>
+      <c r="H27" s="24"/>
+      <c r="I27" s="26"/>
     </row>
     <row r="28" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="8"/>
-      <c r="I28" s="15"/>
+      <c r="A28" s="22"/>
+      <c r="B28" s="24"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="24"/>
+      <c r="H28" s="24"/>
+      <c r="I28" s="26"/>
     </row>
     <row r="29" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="8"/>
-      <c r="I29" s="15"/>
+      <c r="A29" s="23"/>
+      <c r="B29" s="25"/>
+      <c r="C29" s="25"/>
+      <c r="D29" s="25"/>
+      <c r="E29" s="25"/>
+      <c r="F29" s="25"/>
+      <c r="G29" s="25"/>
+      <c r="H29" s="25"/>
+      <c r="I29" s="27"/>
     </row>
     <row r="30" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="8"/>
@@ -2346,6 +2693,22 @@
     <row r="44" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="8"/>
       <c r="I44" s="15"/>
+    </row>
+    <row r="45" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="8"/>
+      <c r="I45" s="15"/>
+    </row>
+    <row r="46" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="8"/>
+      <c r="I46" s="15"/>
+    </row>
+    <row r="47" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="8"/>
+      <c r="I47" s="15"/>
+    </row>
+    <row r="48" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="8"/>
+      <c r="I48" s="15"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>

</xml_diff>